<commit_message>
Home Credit Bank task ready
</commit_message>
<xml_diff>
--- a/Diploma/FullData.xlsx
+++ b/Diploma/FullData.xlsx
@@ -562,10 +562,10 @@
         </is>
       </c>
       <c r="O2" t="n">
-        <v>4439605693.438058</v>
+        <v>694978279716.0918</v>
       </c>
       <c r="P2" t="n">
-        <v>740328503832.2386</v>
+        <v>810790348952.8699</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="O3" t="n">
-        <v>4970729905.609682</v>
+        <v>740020881116.7542</v>
       </c>
       <c r="P3" t="n">
-        <v>828896367849.3679</v>
+        <v>863338907049.2568</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
@@ -672,10 +672,10 @@
         </is>
       </c>
       <c r="O4" t="n">
-        <v>5476189975.55687</v>
+        <v>786493712738.5049</v>
       </c>
       <c r="P4" t="n">
-        <v>913184595942.2444</v>
+        <v>917556030759.684</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
@@ -727,10 +727,10 @@
         </is>
       </c>
       <c r="O5" t="n">
-        <v>5789561285.87219</v>
+        <v>818378053598.4678</v>
       </c>
       <c r="P5" t="n">
-        <v>965440973947.2986</v>
+        <v>954753618952.7168</v>
       </c>
       <c r="Q5" t="n">
         <v>0</v>
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="O6" t="n">
-        <v>6707240710.431314</v>
+        <v>855194498145.8099</v>
       </c>
       <c r="P6" t="n">
-        <v>1118469031458.272</v>
+        <v>997705202898.5314</v>
       </c>
       <c r="Q6" t="n">
         <v>0</v>
@@ -837,10 +837,10 @@
         </is>
       </c>
       <c r="O7" t="n">
-        <v>6095417014.783494</v>
+        <v>6330896320.615259</v>
       </c>
       <c r="P7" t="n">
-        <v>6328669642.154172</v>
+        <v>6358168262.422901</v>
       </c>
       <c r="Q7" t="n">
         <v>0</v>
@@ -892,10 +892,10 @@
         </is>
       </c>
       <c r="O8" t="n">
-        <v>7206607138.351389</v>
+        <v>7462545961.85984</v>
       </c>
       <c r="P8" t="n">
-        <v>7482381551.385285</v>
+        <v>7494692771.553435</v>
       </c>
       <c r="Q8" t="n">
         <v>0</v>
@@ -947,10 +947,10 @@
         </is>
       </c>
       <c r="O9" t="n">
-        <v>8539566041.692849</v>
+        <v>8801934999.328232</v>
       </c>
       <c r="P9" t="n">
-        <v>8866348640.980032</v>
+        <v>8839851567.052563</v>
       </c>
       <c r="Q9" t="n">
         <v>0</v>
@@ -1002,10 +1002,10 @@
         </is>
       </c>
       <c r="O10" t="n">
-        <v>8776840851.317478</v>
+        <v>9064443214.087429</v>
       </c>
       <c r="P10" t="n">
-        <v>9112703218.669683</v>
+        <v>9103490602.535143</v>
       </c>
       <c r="Q10" t="n">
         <v>0</v>
@@ -1057,10 +1057,10 @@
         </is>
       </c>
       <c r="O11" t="n">
-        <v>11740961091.42405</v>
+        <v>12032557931.4547</v>
       </c>
       <c r="P11" t="n">
-        <v>12190251109.77546</v>
+        <v>12084391226.94481</v>
       </c>
       <c r="Q11" t="n">
         <v>0</v>
@@ -1112,10 +1112,10 @@
         </is>
       </c>
       <c r="O12" t="n">
-        <v>6976806.05330259</v>
+        <v>-25817223.80344293</v>
       </c>
       <c r="P12" t="n">
-        <v>454964.4982777229</v>
+        <v>323266.8476926137</v>
       </c>
       <c r="Q12" t="n">
         <v>0</v>
@@ -1167,10 +1167,10 @@
         </is>
       </c>
       <c r="O13" t="n">
-        <v>9439049.625100002</v>
+        <v>-26059103.52738371</v>
       </c>
       <c r="P13" t="n">
-        <v>336283.7564897498</v>
+        <v>320266.295666834</v>
       </c>
       <c r="Q13" t="n">
         <v>0</v>
@@ -1222,10 +1222,10 @@
         </is>
       </c>
       <c r="O14" t="n">
-        <v>10969070.70680849</v>
+        <v>-26525023.32081544</v>
       </c>
       <c r="P14" t="n">
-        <v>289377.2089235937</v>
+        <v>314640.7245027499</v>
       </c>
       <c r="Q14" t="n">
         <v>0</v>
@@ -1277,10 +1277,10 @@
         </is>
       </c>
       <c r="O15" t="n">
-        <v>12040617.41127343</v>
+        <v>-26793968.14207305</v>
       </c>
       <c r="P15" t="n">
-        <v>263624.2774934317</v>
+        <v>311482.5139322564</v>
       </c>
       <c r="Q15" t="n">
         <v>0</v>
@@ -1332,10 +1332,10 @@
         </is>
       </c>
       <c r="O16" t="n">
-        <v>16311391.06199782</v>
+        <v>-27166760.33255523</v>
       </c>
       <c r="P16" t="n">
-        <v>194600.1449880643</v>
+        <v>307208.2373072828</v>
       </c>
       <c r="Q16" t="n">
         <v>0</v>
@@ -1387,10 +1387,10 @@
         </is>
       </c>
       <c r="O17" t="n">
-        <v>-246148222772.6612</v>
+        <v>1070101417468.637</v>
       </c>
       <c r="P17" t="n">
-        <v>206125763991.4501</v>
+        <v>217657887100.7934</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
@@ -1442,10 +1442,10 @@
         </is>
       </c>
       <c r="O18" t="n">
-        <v>-307951051235.0268</v>
+        <v>1244703470703.669</v>
       </c>
       <c r="P18" t="n">
-        <v>257879764447.5222</v>
+        <v>253171823789.6129</v>
       </c>
       <c r="Q18" t="n">
         <v>0</v>
@@ -1497,10 +1497,10 @@
         </is>
       </c>
       <c r="O19" t="n">
-        <v>-354896431764.1998</v>
+        <v>1387310129142.497</v>
       </c>
       <c r="P19" t="n">
-        <v>297192063022.9311</v>
+        <v>282177919338.6917</v>
       </c>
       <c r="Q19" t="n">
         <v>0</v>
@@ -1552,10 +1552,10 @@
         </is>
       </c>
       <c r="O20" t="n">
-        <v>-386382718196.7314</v>
+        <v>1498578330871.818</v>
       </c>
       <c r="P20" t="n">
-        <v>323558838184.064</v>
+        <v>304809794499.8314</v>
       </c>
       <c r="Q20" t="n">
         <v>0</v>
@@ -1607,10 +1607,10 @@
         </is>
       </c>
       <c r="O21" t="n">
-        <v>-503900639256.2129</v>
+        <v>1783215602474.703</v>
       </c>
       <c r="P21" t="n">
-        <v>421968938359.5383</v>
+        <v>362704818388.1016</v>
       </c>
       <c r="Q21" t="n">
         <v>0</v>
@@ -1662,10 +1662,10 @@
         </is>
       </c>
       <c r="O22" t="n">
-        <v>22626085431.96654</v>
+        <v>33817544642.05388</v>
       </c>
       <c r="P22" t="n">
-        <v>22537983732.7454</v>
+        <v>-34988346577.03472</v>
       </c>
       <c r="Q22" t="n">
         <v>0</v>
@@ -1717,10 +1717,10 @@
         </is>
       </c>
       <c r="O23" t="n">
-        <v>17963806220.18574</v>
+        <v>36118448454.44126</v>
       </c>
       <c r="P23" t="n">
-        <v>17893858554.81356</v>
+        <v>-37368910301.58492</v>
       </c>
       <c r="Q23" t="n">
         <v>0</v>
@@ -1772,10 +1772,10 @@
         </is>
       </c>
       <c r="O24" t="n">
-        <v>5704370681.497444</v>
+        <v>34005329284.55395</v>
       </c>
       <c r="P24" t="n">
-        <v>5682158940.472322</v>
+        <v>-35182632537.86307</v>
       </c>
       <c r="Q24" t="n">
         <v>0</v>
@@ -1827,10 +1827,10 @@
         </is>
       </c>
       <c r="O25" t="n">
-        <v>-4254390973.07988</v>
+        <v>33228924401.19743</v>
       </c>
       <c r="P25" t="n">
-        <v>-4237825178.921344</v>
+        <v>-34379347632.63081</v>
       </c>
       <c r="Q25" t="n">
         <v>0</v>
@@ -1882,10 +1882,10 @@
         </is>
       </c>
       <c r="O26" t="n">
-        <v>-11045598047.91013</v>
+        <v>34292900064.32157</v>
       </c>
       <c r="P26" t="n">
-        <v>-11002588577.27674</v>
+        <v>-35480159345.7504</v>
       </c>
       <c r="Q26" t="n">
         <v>0</v>
@@ -1937,13 +1937,13 @@
         </is>
       </c>
       <c r="O27" t="n">
-        <v>-338990599822.0342</v>
+        <v>-836848329799.8755</v>
       </c>
       <c r="P27" t="n">
-        <v>-134280738702.1757</v>
+        <v>-142122415907.5601</v>
       </c>
       <c r="Q27" t="n">
-        <v>199230675509.8303</v>
+        <v>232487190863.3367</v>
       </c>
     </row>
     <row r="28">
@@ -1992,13 +1992,13 @@
         </is>
       </c>
       <c r="O28" t="n">
-        <v>-373414625041.6089</v>
+        <v>-976487825865.4324</v>
       </c>
       <c r="P28" t="n">
-        <v>-131395976818.6101</v>
+        <v>-134784431958.4254</v>
       </c>
       <c r="Q28" t="n">
-        <v>199184115100.8958</v>
+        <v>236893852519.9714</v>
       </c>
     </row>
     <row r="29">
@@ -2047,13 +2047,13 @@
         </is>
       </c>
       <c r="O29" t="n">
-        <v>-406199813999.4192</v>
+        <v>-1093162643918.092</v>
       </c>
       <c r="P29" t="n">
-        <v>-128769831077.4789</v>
+        <v>-129047411966.8208</v>
       </c>
       <c r="Q29" t="n">
-        <v>198095301549.5271</v>
+        <v>238915913219.076</v>
       </c>
     </row>
     <row r="30">
@@ -2102,13 +2102,13 @@
         </is>
       </c>
       <c r="O30" t="n">
-        <v>-442033930346.9777</v>
+        <v>-1197898495125.531</v>
       </c>
       <c r="P30" t="n">
-        <v>-126018005653.4404</v>
+        <v>-124153281187.1788</v>
       </c>
       <c r="Q30" t="n">
-        <v>186200255681.0656</v>
+        <v>229163172706.218</v>
       </c>
     </row>
     <row r="31">
@@ -2157,13 +2157,13 @@
         </is>
       </c>
       <c r="O31" t="n">
-        <v>-498101926934.472</v>
+        <v>-1471794012415.408</v>
       </c>
       <c r="P31" t="n">
-        <v>-121927301493.2948</v>
+        <v>-112284312725.015</v>
       </c>
       <c r="Q31" t="n">
-        <v>179807841968.7111</v>
+        <v>230549023295.8817</v>
       </c>
     </row>
     <row r="32">
@@ -2212,10 +2212,10 @@
         </is>
       </c>
       <c r="O32" t="n">
-        <v>579520008.5356214</v>
+        <v>535869327.7461484</v>
       </c>
       <c r="P32" t="n">
-        <v>579520008.5356214</v>
+        <v>4980412425.635483</v>
       </c>
       <c r="Q32" t="n">
         <v>0</v>
@@ -2267,10 +2267,10 @@
         </is>
       </c>
       <c r="O33" t="n">
-        <v>562315883.9901829</v>
+        <v>575689332.9933953</v>
       </c>
       <c r="P33" t="n">
-        <v>562315883.9901829</v>
+        <v>5350502741.788466</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
@@ -2322,10 +2322,10 @@
         </is>
       </c>
       <c r="O34" t="n">
-        <v>457214037.0223798</v>
+        <v>550760905.9213717</v>
       </c>
       <c r="P34" t="n">
-        <v>457214037.0223798</v>
+        <v>5118815945.189672</v>
       </c>
       <c r="Q34" t="n">
         <v>0</v>
@@ -2377,10 +2377,10 @@
         </is>
       </c>
       <c r="O35" t="n">
-        <v>374064825.8799433</v>
+        <v>545025824.1063117</v>
       </c>
       <c r="P35" t="n">
-        <v>374064825.8799433</v>
+        <v>5065513635.736925</v>
       </c>
       <c r="Q35" t="n">
         <v>0</v>
@@ -2432,10 +2432,10 @@
         </is>
       </c>
       <c r="O36" t="n">
-        <v>311043387.9822282</v>
+        <v>564818736.920082</v>
       </c>
       <c r="P36" t="n">
-        <v>311043387.9822282</v>
+        <v>5249470551.748209</v>
       </c>
       <c r="Q36" t="n">
         <v>0</v>
@@ -2487,13 +2487,13 @@
         </is>
       </c>
       <c r="O37" t="n">
-        <v>572714348093.0168</v>
+        <v>1493155485025.285</v>
       </c>
       <c r="P37" t="n">
-        <v>700928502260.9518</v>
+        <v>699741525770.7982</v>
       </c>
       <c r="Q37" t="n">
-        <v>3.996265672480812e-11</v>
+        <v>4.137711712503987e-11</v>
       </c>
     </row>
     <row r="38">
@@ -2542,13 +2542,13 @@
         </is>
       </c>
       <c r="O38" t="n">
-        <v>665427076450.3153</v>
+        <v>1816099117008.94</v>
       </c>
       <c r="P38" t="n">
-        <v>704813042786.0435</v>
+        <v>704629127768.343</v>
       </c>
       <c r="Q38" t="n">
-        <v>3.929261316673382e-11</v>
+        <v>4.07417351541515e-11</v>
       </c>
     </row>
     <row r="39">
@@ -2597,13 +2597,13 @@
         </is>
       </c>
       <c r="O39" t="n">
-        <v>743531494971.6614</v>
+        <v>2067931981765.103</v>
       </c>
       <c r="P39" t="n">
-        <v>707686334278.5715</v>
+        <v>707870689643.0153</v>
       </c>
       <c r="Q39" t="n">
-        <v>3.865982429290243e-11</v>
+        <v>4.010651679141045e-11</v>
       </c>
     </row>
     <row r="40">
@@ -2652,13 +2652,13 @@
         </is>
       </c>
       <c r="O40" t="n">
-        <v>807874040486.4841</v>
+        <v>2250696813230.056</v>
       </c>
       <c r="P40" t="n">
-        <v>709835049953.9095</v>
+        <v>709984768283.6155</v>
       </c>
       <c r="Q40" t="n">
-        <v>3.773899555456663e-11</v>
+        <v>3.91492888574885e-11</v>
       </c>
     </row>
     <row r="41">
@@ -2707,13 +2707,13 @@
         </is>
       </c>
       <c r="O41" t="n">
-        <v>977817995237.4459</v>
+        <v>2854854410876.348</v>
       </c>
       <c r="P41" t="n">
-        <v>714777842350.9967</v>
+        <v>715920332871.3195</v>
       </c>
       <c r="Q41" t="n">
-        <v>3.74729754475317e-11</v>
+        <v>3.892725170109283e-11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>